<commit_message>
clean the inappropriate COUNTERPARTY_NOT_STATED in amount column
</commit_message>
<xml_diff>
--- a/Raw Input Data/Processing/Case 10/Suspect 3 txn report.xlsx
+++ b/Raw Input Data/Processing/Case 10/Suspect 3 txn report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hbap.adroot.hsbc\HK\HASE\28062201\Fraud_Ops_FIM_File_Sharing\HASE case\Gen AI\Masked case (Edwin)\Batch 1\Case 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Processing\Case 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A8E0F7-7A90-475A-B4C4-A26B32151732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA64213-FF31-4C2B-8E8B-1FD4D3E7F627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10950" yWindow="-21330" windowWidth="31470" windowHeight="20235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27240" yWindow="6810" windowWidth="20520" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction record" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Transaction Date (value)</t>
   </si>
@@ -155,13 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,122 +473,121 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>45434</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2">
+        <v>50000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2">
         <v>50000</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2">
         <v>2</v>
       </c>
     </row>
@@ -603,6 +601,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A8F4FDE63F23240996C0B5ED71CAB02" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61b2ee7a38442529347de99e33b69841">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc14db02-3d39-436b-9056-63d1dbe054e8" xmlns:ns3="5ed3fcfa-dd51-4f96-90c6-6669337cd654" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="405649729e347460199c909c216f19f3" ns2:_="" ns3:_="">
     <xsd:import namespace="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
@@ -797,34 +815,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7211D5B4-69EE-4214-A93B-1197871E056A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB219326-B5C3-4152-9DE8-2279BD89FA76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00B0F5A6-F3C1-4A7A-ADDC-083A7C82B6B4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00B0F5A6-F3C1-4A7A-ADDC-083A7C82B6B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB219326-B5C3-4152-9DE8-2279BD89FA76}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7211D5B4-69EE-4214-A93B-1197871E056A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>